<commit_message>
Added prototype rubber band bots
See rubber_band_bot v1 > prototype_robot and prototype robot_phase2_WORKS. These programs simulate the functions of my rubber band robot while only using a button and an ultrasonic rangefinder
</commit_message>
<xml_diff>
--- a/rubber_band_bot v1/more info/Rubber band experimental data.xlsx
+++ b/rubber_band_bot v1/more info/Rubber band experimental data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nufer PC\Documents\Kevin\Arduino\Robotics Merit badge\Code\Elegoo-Robot-Car-master\rubber_band_bot\more info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nufer PC\Documents\GitHub\Elegoo-Robot-Car\rubber_band_bot v1\more info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2812,6 +2812,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2886,7 +2890,7 @@
         <v>2.875</v>
       </c>
       <c r="G5">
-        <f>F5-$F$5</f>
+        <f t="shared" ref="G5:G19" si="0">F5-$F$5</f>
         <v>0</v>
       </c>
     </row>
@@ -2911,11 +2915,11 @@
         <v>3.25</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F19" si="0">AVERAGE(C6:E6)</f>
+        <f t="shared" ref="F6:F19" si="1">AVERAGE(C6:E6)</f>
         <v>3.25</v>
       </c>
       <c r="G6">
-        <f>F6-$F$5</f>
+        <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
     </row>
@@ -2924,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B19" si="1">A7*$B$1</f>
+        <f t="shared" ref="B7:B19" si="2">A7*$B$1</f>
         <v>0.77500000000000002</v>
       </c>
       <c r="C7">
@@ -2940,11 +2944,11 @@
         <v>3.875</v>
       </c>
       <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.020833333333333</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>4.020833333333333</v>
-      </c>
-      <c r="G7">
-        <f>F7-$F$5</f>
         <v>1.145833333333333</v>
       </c>
     </row>
@@ -2953,7 +2957,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1625000000000001</v>
       </c>
       <c r="C8">
@@ -2968,11 +2972,11 @@
         <v>5.5</v>
       </c>
       <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.229166666666667</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>6.229166666666667</v>
-      </c>
-      <c r="G8">
-        <f>F8-$F$5</f>
         <v>3.354166666666667</v>
       </c>
     </row>
@@ -2981,7 +2985,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.55</v>
       </c>
       <c r="C9">
@@ -2996,11 +3000,11 @@
         <v>9</v>
       </c>
       <c r="F9">
+        <f t="shared" si="1"/>
+        <v>9.4583333333333339</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>9.4583333333333339</v>
-      </c>
-      <c r="G9">
-        <f>F9-$F$5</f>
         <v>6.5833333333333339</v>
       </c>
     </row>
@@ -3009,7 +3013,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9375</v>
       </c>
       <c r="C10">
@@ -3024,11 +3028,11 @@
         <v>11.125</v>
       </c>
       <c r="F10">
+        <f t="shared" si="1"/>
+        <v>12.0625</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>12.0625</v>
-      </c>
-      <c r="G10">
-        <f>F10-$F$5</f>
         <v>9.1875</v>
       </c>
     </row>
@@ -3037,7 +3041,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3250000000000002</v>
       </c>
       <c r="C11">
@@ -3053,11 +3057,11 @@
         <v>12.625</v>
       </c>
       <c r="F11">
+        <f t="shared" si="1"/>
+        <v>13.708333333333334</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>13.708333333333334</v>
-      </c>
-      <c r="G11">
-        <f>F11-$F$5</f>
         <v>10.833333333333334</v>
       </c>
     </row>
@@ -3066,7 +3070,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7124999999999999</v>
       </c>
       <c r="C12">
@@ -3082,11 +3086,11 @@
         <v>13.75</v>
       </c>
       <c r="F12">
+        <f t="shared" si="1"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>14.666666666666666</v>
-      </c>
-      <c r="G12">
-        <f>F12-$F$5</f>
         <v>11.791666666666666</v>
       </c>
     </row>
@@ -3095,7 +3099,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
       <c r="C13">
@@ -3110,11 +3114,11 @@
         <v>14.5</v>
       </c>
       <c r="F13">
+        <f t="shared" si="1"/>
+        <v>15.416666666666666</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>15.416666666666666</v>
-      </c>
-      <c r="G13">
-        <f>F13-$F$5</f>
         <v>12.541666666666666</v>
       </c>
     </row>
@@ -3123,7 +3127,7 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4875000000000003</v>
       </c>
       <c r="C14">
@@ -3139,11 +3143,11 @@
         <v>15.125</v>
       </c>
       <c r="F14">
+        <f t="shared" si="1"/>
+        <v>16.083333333333332</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>16.083333333333332</v>
-      </c>
-      <c r="G14">
-        <f>F14-$F$5</f>
         <v>13.208333333333332</v>
       </c>
     </row>
@@ -3152,7 +3156,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.875</v>
       </c>
       <c r="C15">
@@ -3167,11 +3171,11 @@
         <v>15.5</v>
       </c>
       <c r="F15">
+        <f t="shared" si="1"/>
+        <v>16.458333333333332</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="0"/>
-        <v>16.458333333333332</v>
-      </c>
-      <c r="G15">
-        <f>F15-$F$5</f>
         <v>13.583333333333332</v>
       </c>
     </row>
@@ -3180,7 +3184,7 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2625000000000002</v>
       </c>
       <c r="C16">
@@ -3196,11 +3200,11 @@
         <v>16.25</v>
       </c>
       <c r="F16">
+        <f t="shared" si="1"/>
+        <v>17.041666666666668</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="0"/>
-        <v>17.041666666666668</v>
-      </c>
-      <c r="G16">
-        <f>F16-$F$5</f>
         <v>14.166666666666668</v>
       </c>
     </row>
@@ -3209,7 +3213,7 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6500000000000004</v>
       </c>
       <c r="C17">
@@ -3224,11 +3228,11 @@
         <v>16.375</v>
       </c>
       <c r="F17">
+        <f t="shared" si="1"/>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
-        <v>17.333333333333332</v>
-      </c>
-      <c r="G17">
-        <f>F17-$F$5</f>
         <v>14.458333333333332</v>
       </c>
     </row>
@@ -3237,7 +3241,7 @@
         <v>13</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0375000000000005</v>
       </c>
       <c r="C18">
@@ -3252,11 +3256,11 @@
         <v>16.875</v>
       </c>
       <c r="F18">
+        <f t="shared" si="1"/>
+        <v>17.708333333333332</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="0"/>
-        <v>17.708333333333332</v>
-      </c>
-      <c r="G18">
-        <f>F18-$F$5</f>
         <v>14.833333333333332</v>
       </c>
     </row>
@@ -3265,7 +3269,7 @@
         <v>14</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.4249999999999998</v>
       </c>
       <c r="C19">
@@ -3281,11 +3285,11 @@
         <v>17.25</v>
       </c>
       <c r="F19">
+        <f t="shared" si="1"/>
+        <v>18.083333333333332</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
-        <v>18.083333333333332</v>
-      </c>
-      <c r="G19">
-        <f>F19-$F$5</f>
         <v>15.208333333333332</v>
       </c>
     </row>

</xml_diff>